<commit_message>
additions to refinement scheme
</commit_message>
<xml_diff>
--- a/models/dft/hecs_for_approx/properties.xlsx
+++ b/models/dft/hecs_for_approx/properties.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="2" r:id="rId1"/>
+    <sheet name="Properties few" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>failed</t>
   </si>
@@ -342,7 +343,7 @@
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A1:A26"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,4 +481,34 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>16000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>